<commit_message>
head counter refresh. FZM's code testing.
</commit_message>
<xml_diff>
--- a/MyFlower/reports/stage-1-table.xlsx
+++ b/MyFlower/reports/stage-1-table.xlsx
@@ -48,10 +48,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Foreground SPP Pooling+Raw Image(Late Fusion)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Foreground SPP Pooling+Background Image(Early Fusion)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -102,6 +98,10 @@
   </si>
   <si>
     <t>BENCHMARK:BiCoS: A Bi-level Co-Segmentation Method for Image Classification</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Foreground SPP Pooling+Raw Image(Late Fusion)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -613,11 +613,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="1231243344"/>
-        <c:axId val="1231247152"/>
+        <c:axId val="-2094496800"/>
+        <c:axId val="-2094487552"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1231243344"/>
+        <c:axId val="-2094496800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -660,7 +660,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1231247152"/>
+        <c:crossAx val="-2094487552"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -668,7 +668,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1231247152"/>
+        <c:axId val="-2094487552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -719,7 +719,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1231243344"/>
+        <c:crossAx val="-2094496800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1690,7 +1690,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1702,13 +1702,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
@@ -1790,7 +1790,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2">
         <v>82.598799999999997</v>
@@ -1812,7 +1812,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="B11" s="5">
         <v>83.37</v>
@@ -1823,7 +1823,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A12" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" s="2">
         <v>82.875299999999996</v>
@@ -1834,7 +1834,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B13" s="2">
         <v>64.14</v>
@@ -1845,7 +1845,7 @@
     </row>
     <row r="14" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B14" s="2">
         <v>73.3</v>
@@ -1856,10 +1856,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="2">
         <v>28.2</v>
@@ -1867,7 +1867,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B16" s="2">
         <v>80</v>
@@ -1883,19 +1883,19 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A19" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Myflower gao model finished.
</commit_message>
<xml_diff>
--- a/MyFlower/reports/stage-1-table.xlsx
+++ b/MyFlower/reports/stage-1-table.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Foreground Only</t>
     <phoneticPr fontId="3" type="noConversion"/>
@@ -84,7 +84,15 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>BENCHMARK: unsupervised template learning for fine-grained object ecognition</t>
+    <t>除了SPP和原图组合中，late fusion效果比early 效果好以外，其他的fusion策略都是early fusion好(这一点很奇怪！）</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Foreground SPP Pooling+Raw Image(Late Fusion)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gao</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -93,15 +101,11 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>除了SPP和原图组合中，late fusion效果比early 效果好以外，其他的fusion策略都是early fusion好(这一点很奇怪！）</t>
+    <t>BENCHMARK: unsupervised template learning for fine-grained object ecognition</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>BENCHMARK:BiCoS: A Bi-level Co-Segmentation Method for Image Classification</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Foreground SPP Pooling+Raw Image(Late Fusion)</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -613,11 +617,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="100"/>
-        <c:axId val="-2094496800"/>
-        <c:axId val="-2094487552"/>
+        <c:axId val="1676497744"/>
+        <c:axId val="1676499920"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2094496800"/>
+        <c:axId val="1676497744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -660,7 +664,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2094487552"/>
+        <c:crossAx val="1676499920"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -668,7 +672,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2094487552"/>
+        <c:axId val="1676499920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -719,7 +723,7 @@
             <a:endParaRPr lang="zh-CN"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2094496800"/>
+        <c:crossAx val="1676497744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1369,15 +1373,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>9526</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>76201</xdr:colOff>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>61912</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>333376</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>400051</xdr:colOff>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1690,7 +1694,7 @@
   <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1812,7 +1816,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B11" s="5">
         <v>83.37</v>
@@ -1845,7 +1849,7 @@
     </row>
     <row r="14" spans="1:3" ht="27" x14ac:dyDescent="0.15">
       <c r="A14" s="6" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B14" s="2">
         <v>73.3</v>
@@ -1856,7 +1860,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A15" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>16</v>
@@ -1867,7 +1871,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A16" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B16" s="2">
         <v>80</v>
@@ -1877,9 +1881,15 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
+      <c r="A17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="5">
+        <v>87.64</v>
+      </c>
+      <c r="C17" s="5">
+        <v>41.83</v>
+      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A18" s="2" t="s">
@@ -1895,7 +1905,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>